<commit_message>
flipped connector on module
</commit_message>
<xml_diff>
--- a/Paperino_module/BOM/paperino BOM.xlsx
+++ b/Paperino_module/BOM/paperino BOM.xlsx
@@ -105,12 +105,6 @@
     <t>C3, C4</t>
   </si>
   <si>
-    <t>C5, C6, C7, C8</t>
-  </si>
-  <si>
-    <t>C1, C2, C9</t>
-  </si>
-  <si>
     <t>Cap 2µ2/35V</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t>SOT-23</t>
+  </si>
+  <si>
+    <t>C1, C2, C5</t>
+  </si>
+  <si>
+    <t>C6, C7, C8, C9</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,16 +558,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -587,12 +587,12 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -607,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -689,10 +689,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -701,70 +701,70 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8">
         <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>